<commit_message>
v0.0.6 Improved all files and added other tests
</commit_message>
<xml_diff>
--- a/docs/feasibility/Map_to_Geojson_Gantt.xlsx
+++ b/docs/feasibility/Map_to_Geojson_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\Map_to_Geojson-Converter\docs\feasibility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626267C6-76E0-44C2-A62B-90B77B3BE113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE1D6AC-97B9-428E-8B9D-D0EE36F185DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{9327F8D6-4F37-4E25-8083-20A17765DC2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9327F8D6-4F37-4E25-8083-20A17765DC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,18 +42,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
-    <t>Map to .geojson</t>
-  </si>
-  <si>
     <t>Project Start: 6 October 2025</t>
   </si>
   <si>
     <t>Month</t>
   </si>
   <si>
-    <t>Gantt v1.0.0</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -87,93 +81,27 @@
     <t>END</t>
   </si>
   <si>
-    <t>Progettazzione del prototipo</t>
-  </si>
-  <si>
-    <t>Studio di fattibilità</t>
-  </si>
-  <si>
     <t>F,M,L</t>
   </si>
   <si>
-    <t>Progettazione Gantt</t>
-  </si>
-  <si>
     <t>M,L</t>
   </si>
   <si>
-    <t>Studio svg e geojson</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t xml:space="preserve">  Studio dataset</t>
-  </si>
-  <si>
     <t>F,L</t>
   </si>
   <si>
-    <t>Prototipo svg to geojson-converter</t>
-  </si>
-  <si>
-    <t>Introduzione dell AI</t>
-  </si>
-  <si>
-    <t>Ricerca del dataset</t>
-  </si>
-  <si>
-    <t>Ricerca del modello pre-trained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Implementazione del modello</t>
-  </si>
-  <si>
-    <t>fine-tuning del modello</t>
-  </si>
-  <si>
-    <t>UI</t>
-  </si>
-  <si>
-    <t>Progettazione figma</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>Implementazione front-end</t>
-  </si>
-  <si>
-    <t>Test Finale</t>
-  </si>
-  <si>
-    <t>Test del modello</t>
-  </si>
-  <si>
-    <t>Test finale progetto + front-end</t>
-  </si>
-  <si>
-    <t>Rilascio della beta e test degli utenti</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marketing </t>
   </si>
   <si>
-    <t>Studio del brand</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
-    <t xml:space="preserve">Progettazione dell'entrata in mercato </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Progettazione marketing </t>
-  </si>
-  <si>
-    <t>Componenti:</t>
-  </si>
-  <si>
     <t>Fabio Ferro</t>
   </si>
   <si>
@@ -199,6 +127,78 @@
   </si>
   <si>
     <t>Costo Risorse Esterne:</t>
+  </si>
+  <si>
+    <t>Gantt v3.0.0</t>
+  </si>
+  <si>
+    <t>Map to .geojson converter</t>
+  </si>
+  <si>
+    <t>Collaborators</t>
+  </si>
+  <si>
+    <t>Research &amp; Prototyping</t>
+  </si>
+  <si>
+    <t>Feasibility Study</t>
+  </si>
+  <si>
+    <t>Gantt Prototype</t>
+  </si>
+  <si>
+    <t>SVG &amp; GeoJSON study</t>
+  </si>
+  <si>
+    <t>Dataset Study</t>
+  </si>
+  <si>
+    <t>SVG to GeoJSON protype</t>
+  </si>
+  <si>
+    <t>Dataset Research</t>
+  </si>
+  <si>
+    <t>Computer Vision Development</t>
+  </si>
+  <si>
+    <t>Libraries Research</t>
+  </si>
+  <si>
+    <t>Initial Implementation</t>
+  </si>
+  <si>
+    <t>More Features</t>
+  </si>
+  <si>
+    <t>UI Development</t>
+  </si>
+  <si>
+    <t>Figma design</t>
+  </si>
+  <si>
+    <t>Front-end implementation</t>
+  </si>
+  <si>
+    <t>Testing &amp; Release</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Testing + UI</t>
+  </si>
+  <si>
+    <t>Beta release and user testing</t>
+  </si>
+  <si>
+    <t>Brand study</t>
+  </si>
+  <si>
+    <t>Market entry planning</t>
+  </si>
+  <si>
+    <t>Marketing planning</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1066,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490757F6-93EC-4607-8435-BB8805CD3E41}">
   <dimension ref="C2:AU41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E12" sqref="E12"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1088,18 +1088,18 @@
   <sheetData>
     <row r="2" spans="3:47" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="62" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D2" s="62"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C3" s="60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="60"/>
       <c r="H3" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3" s="61" t="str">
         <f>TEXT(I5,"MMM")</f>
@@ -1166,10 +1166,10 @@
     </row>
     <row r="4" spans="3:47" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="5" spans="3:47" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I5" s="11">
         <v>45936</v>
@@ -1390,30 +1390,30 @@
         <v>46174</v>
       </c>
       <c r="AS5" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT5" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU5" s="50" t="s">
         <v>7</v>
-      </c>
-      <c r="AT5" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU5" s="50" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="F6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="G6" s="37" t="s">
         <v>12</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="37" t="s">
-        <v>14</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="7" spans="3:47" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="34" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="28"/>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="8" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="33" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E8" s="27">
         <v>1</v>
@@ -1573,10 +1573,10 @@
     </row>
     <row r="9" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="33" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E9" s="27">
         <v>1</v>
@@ -1638,13 +1638,13 @@
     </row>
     <row r="10" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="33" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E10" s="27">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="F10" s="30">
         <v>45955</v>
@@ -1703,10 +1703,10 @@
     </row>
     <row r="11" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="33" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E11" s="27">
         <v>0.2</v>
@@ -1768,10 +1768,10 @@
     </row>
     <row r="12" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="33" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E12" s="27">
         <v>0</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="13" spans="3:47" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="35" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="31"/>
@@ -1890,10 +1890,10 @@
     </row>
     <row r="14" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="33" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E14" s="27">
         <v>0.2</v>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="15" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="33" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E15" s="27">
         <v>0.2</v>
@@ -2020,10 +2020,10 @@
     </row>
     <row r="16" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="33" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E16" s="27">
         <v>0</v>
@@ -2085,10 +2085,10 @@
     </row>
     <row r="17" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="33" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E17" s="27">
         <v>0</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="18" spans="3:47" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="35" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="31"/>
@@ -2207,10 +2207,10 @@
     </row>
     <row r="19" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="33" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E19" s="27">
         <v>0</v>
@@ -2272,10 +2272,10 @@
     </row>
     <row r="20" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="33" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E20" s="27">
         <v>0</v>
@@ -2337,7 +2337,7 @@
     </row>
     <row r="21" spans="3:47" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="35" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D21" s="35"/>
       <c r="E21" s="31"/>
@@ -2394,10 +2394,10 @@
     </row>
     <row r="22" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="33" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E22" s="27">
         <v>0</v>
@@ -2459,10 +2459,10 @@
     </row>
     <row r="23" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="33" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E23" s="27">
         <v>0</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="24" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="33" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D24" s="33"/>
       <c r="E24" s="26"/>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="25" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="35" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="31"/>
@@ -2642,13 +2642,13 @@
     </row>
     <row r="26" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="33" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E26" s="27">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F26" s="30">
         <v>45969</v>
@@ -2707,10 +2707,10 @@
     </row>
     <row r="27" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="33" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
@@ -2772,10 +2772,10 @@
     </row>
     <row r="28" spans="3:47" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="33" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E28" s="27">
         <v>0</v>
@@ -2856,10 +2856,10 @@
     </row>
     <row r="32" spans="3:47" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="C32" s="46" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E32" s="58"/>
       <c r="F32" s="59"/>
@@ -2879,7 +2879,7 @@
     <row r="33" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C33" s="43"/>
       <c r="D33" s="58" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="E33" s="58"/>
       <c r="F33" s="59"/>
@@ -2887,7 +2887,7 @@
     <row r="34" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C34" s="43"/>
       <c r="D34" s="58" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E34" s="58"/>
       <c r="F34" s="59"/>
@@ -2898,7 +2898,7 @@
     <row r="35" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C35" s="43"/>
       <c r="D35" s="58" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="E35" s="58"/>
       <c r="F35" s="59"/>
@@ -2926,13 +2926,13 @@
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C38" s="51" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D38" s="47">
         <v>3</v>
       </c>
       <c r="E38" s="38" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F38" s="42"/>
       <c r="J38" s="2"/>
@@ -2941,13 +2941,13 @@
     </row>
     <row r="39" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C39" s="51" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D39" s="47">
         <v>15</v>
       </c>
       <c r="E39" s="38" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="F39" s="42"/>
       <c r="J39" s="2"/>
@@ -2956,13 +2956,13 @@
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C40" s="51" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D40">
         <v>25</v>
       </c>
       <c r="E40" s="38" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="F40" s="48"/>
     </row>

</xml_diff>